<commit_message>
Update Alert Parameters (working).xlsx
</commit_message>
<xml_diff>
--- a/alerts/Alert Parameters (working).xlsx
+++ b/alerts/Alert Parameters (working).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztsmith\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztsmith\Documents\GitHub\CEVAC\alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>Alert</t>
   </si>
@@ -113,12 +113,6 @@
     <t>null/empty</t>
   </si>
   <si>
-    <t>IAQ</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Emergency</t>
   </si>
   <si>
@@ -129,6 +123,42 @@
   </si>
   <si>
     <t>1000 warn, 2000 alarm</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEVAC_x_POWER_LATEST </t>
+  </si>
+  <si>
+    <t>CEVAC_x_TEMP_LATEST</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Value in table</t>
+  </si>
+  <si>
+    <t>All rooms</t>
+  </si>
+  <si>
+    <t>sum of all actualvalue</t>
+  </si>
+  <si>
+    <t>Building Lighting actualvalue</t>
+  </si>
+  <si>
+    <t>sum of 3rd floor emergency and basement emergency</t>
+  </si>
+  <si>
+    <t>CEVAC_x_IAQ_LATEST</t>
+  </si>
+  <si>
+    <t>all sensors</t>
   </si>
 </sst>
 </file>
@@ -176,12 +206,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,18 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +525,14 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -509,8 +548,11 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -526,8 +568,11 @@
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -543,8 +588,14 @@
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -563,8 +614,14 @@
       <c r="F5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -580,8 +637,11 @@
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -597,8 +657,11 @@
       <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -614,8 +677,14 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -631,8 +700,14 @@
       <c r="E9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -648,78 +723,71 @@
       <c r="E10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>